<commit_message>
Armases in R data
</commit_message>
<xml_diff>
--- a/rawdata/Site_data.xlsx
+++ b/rawdata/Site_data.xlsx
@@ -1,18 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weitinglin/Dropbox/PhD_projects/iva_latitude/rawdata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
     <sheet name="site_notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -569,19 +580,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -589,14 +600,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -635,6 +646,22 @@
       <color rgb="FF000000"/>
       <name val="AdvP403A40"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -656,10 +683,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,15 +695,17 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -706,10 +735,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1024,20 +1055,21 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection sqref="A1:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" customHeight="1">
+    <row r="1" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1089,7 +1121,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="16.5">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1112,7 +1144,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="16.5">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1137,7 +1169,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="16.5">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1162,7 +1194,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="16.5">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1185,7 +1217,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="16.5">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1212,7 +1244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16.5">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1235,7 +1267,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="16.5">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>173</v>
       </c>
@@ -1262,7 +1294,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16.5">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1285,7 +1317,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="16.5">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1310,7 +1342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -1335,7 +1367,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="16.5">
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1360,7 +1392,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="20.25" customHeight="1">
+    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>22</v>
       </c>
@@ -1387,7 +1419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.5">
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1414,7 +1446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.5">
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1456,15 +1488,15 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.95" customHeight="1">
+    <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
@@ -1487,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.95" customHeight="1">
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -1508,7 +1540,7 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.95" customHeight="1">
+    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -1529,7 +1561,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.95" customHeight="1">
+    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1550,7 +1582,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.95" customHeight="1">
+    <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>34</v>
       </c>
@@ -1571,7 +1603,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.95" customHeight="1">
+    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -1592,7 +1624,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.95" customHeight="1">
+    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
@@ -1613,7 +1645,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.95" customHeight="1">
+    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1634,7 +1666,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.95" customHeight="1">
+    <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
@@ -1655,7 +1687,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15.95" customHeight="1">
+    <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -1676,7 +1708,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.95" customHeight="1">
+    <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1729,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.95" customHeight="1">
+    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
@@ -1718,7 +1750,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15.95" customHeight="1">
+    <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
@@ -1739,7 +1771,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.95" customHeight="1">
+    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
@@ -1760,7 +1792,7 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15.95" customHeight="1">
+    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
@@ -1781,7 +1813,7 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.95" customHeight="1">
+    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -1802,7 +1834,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="15.95" customHeight="1">
+    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>81</v>
       </c>
@@ -1823,7 +1855,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15.95" customHeight="1">
+    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>81</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="15.95" customHeight="1">
+    <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>81</v>
       </c>
@@ -1865,7 +1897,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15.95" customHeight="1">
+    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>81</v>
       </c>
@@ -1888,7 +1920,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.95" customHeight="1">
+    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>81</v>
       </c>
@@ -1909,7 +1941,7 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="15.95" customHeight="1">
+    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>81</v>
       </c>
@@ -1930,7 +1962,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="15.95" customHeight="1">
+    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>81</v>
       </c>
@@ -1951,7 +1983,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15.95" customHeight="1">
+    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>81</v>
       </c>
@@ -1972,7 +2004,7 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="15.95" customHeight="1">
+    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>81</v>
       </c>
@@ -1993,7 +2025,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="15.95" customHeight="1">
+    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>81</v>
       </c>
@@ -2014,7 +2046,7 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15.95" customHeight="1">
+    <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>81</v>
       </c>
@@ -2035,7 +2067,7 @@
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15.95" customHeight="1">
+    <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>81</v>
       </c>
@@ -2056,7 +2088,7 @@
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="15.95" customHeight="1">
+    <row r="29" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>81</v>
       </c>
@@ -2077,7 +2109,7 @@
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="15.95" customHeight="1">
+    <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>81</v>
       </c>
@@ -2098,7 +2130,7 @@
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="15.95" customHeight="1">
+    <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>81</v>
       </c>
@@ -2119,7 +2151,7 @@
       </c>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15.95" customHeight="1">
+    <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>81</v>
       </c>
@@ -2140,7 +2172,7 @@
       </c>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="15.95" customHeight="1">
+    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>81</v>
       </c>
@@ -2161,7 +2193,7 @@
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="15.95" customHeight="1">
+    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>81</v>
       </c>
@@ -2182,7 +2214,7 @@
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15.95" customHeight="1">
+    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>81</v>
       </c>
@@ -2203,7 +2235,7 @@
       </c>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="15.95" customHeight="1">
+    <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>81</v>
       </c>
@@ -2224,7 +2256,7 @@
       </c>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15.95" customHeight="1">
+    <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>81</v>
       </c>
@@ -2245,7 +2277,7 @@
       </c>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="15.95" customHeight="1">
+    <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>81</v>
       </c>
@@ -2266,7 +2298,7 @@
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" ht="15.95" customHeight="1">
+    <row r="39" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>81</v>
       </c>
@@ -2287,7 +2319,7 @@
       </c>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7" ht="15.95" customHeight="1">
+    <row r="40" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>81</v>
       </c>

</xml_diff>